<commit_message>
Changes made on day 14 Aug 2024
</commit_message>
<xml_diff>
--- a/Data Files/dataFile.xlsx
+++ b/Data Files/dataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>User Name</t>
   </si>
@@ -55,6 +55,132 @@
   </si>
   <si>
     <t>Test11082024@125</t>
+  </si>
+  <si>
+    <t>Test12082024@221.com</t>
+  </si>
+  <si>
+    <t>Test12082024@221</t>
+  </si>
+  <si>
+    <t>Test12082024@421.com</t>
+  </si>
+  <si>
+    <t>Test12082024@421</t>
+  </si>
+  <si>
+    <t>Test12082024@590.com</t>
+  </si>
+  <si>
+    <t>Test12082024@590</t>
+  </si>
+  <si>
+    <t>Test12082024@584.com</t>
+  </si>
+  <si>
+    <t>Test12082024@584</t>
+  </si>
+  <si>
+    <t>Test13082024@458.com</t>
+  </si>
+  <si>
+    <t>Test13082024@458</t>
+  </si>
+  <si>
+    <t>Test13082024@681.com</t>
+  </si>
+  <si>
+    <t>Test13082024@681</t>
+  </si>
+  <si>
+    <t>Test13082024@266.com</t>
+  </si>
+  <si>
+    <t>Test13082024@266</t>
+  </si>
+  <si>
+    <t>Test13082024@361.com</t>
+  </si>
+  <si>
+    <t>Test13082024@361</t>
+  </si>
+  <si>
+    <t>Test13082024@939.com</t>
+  </si>
+  <si>
+    <t>Test13082024@939</t>
+  </si>
+  <si>
+    <t>Test13082024@301.com</t>
+  </si>
+  <si>
+    <t>Test13082024@301</t>
+  </si>
+  <si>
+    <t>Test13082024@977.com</t>
+  </si>
+  <si>
+    <t>Test13082024@977</t>
+  </si>
+  <si>
+    <t>Test13082024@942.com</t>
+  </si>
+  <si>
+    <t>Test13082024@942</t>
+  </si>
+  <si>
+    <t>Test13082024@973.com</t>
+  </si>
+  <si>
+    <t>Test13082024@973</t>
+  </si>
+  <si>
+    <t>Test13082024@848.com</t>
+  </si>
+  <si>
+    <t>Test13082024@848</t>
+  </si>
+  <si>
+    <t>Test13082024@763.com</t>
+  </si>
+  <si>
+    <t>Test13082024@763</t>
+  </si>
+  <si>
+    <t>Test13082024@945.com</t>
+  </si>
+  <si>
+    <t>Test13082024@945</t>
+  </si>
+  <si>
+    <t>Test13082024@604.com</t>
+  </si>
+  <si>
+    <t>Test13082024@604</t>
+  </si>
+  <si>
+    <t>Test13082024@366.com</t>
+  </si>
+  <si>
+    <t>Test13082024@366</t>
+  </si>
+  <si>
+    <t>Test13082024@269.com</t>
+  </si>
+  <si>
+    <t>Test13082024@269</t>
+  </si>
+  <si>
+    <t>Test13082024@0.com</t>
+  </si>
+  <si>
+    <t>Test13082024@0</t>
+  </si>
+  <si>
+    <t>Test14082024@724.com</t>
+  </si>
+  <si>
+    <t>Test14082024@724</t>
   </si>
 </sst>
 </file>
@@ -414,10 +540,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3"/>
     </row>

</xml_diff>

<commit_message>
Committing changes for cache removed 14/08/2024
</commit_message>
<xml_diff>
--- a/Data Files/dataFile.xlsx
+++ b/Data Files/dataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>User Name</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>Test14082024@724</t>
+  </si>
+  <si>
+    <t>Test14082024@953.com</t>
+  </si>
+  <si>
+    <t>Test14082024@953</t>
+  </si>
+  <si>
+    <t>Test14082024@657.com</t>
+  </si>
+  <si>
+    <t>Test14082024@657</t>
   </si>
 </sst>
 </file>
@@ -540,10 +552,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3"/>
     </row>

</xml_diff>

<commit_message>
Commit for the 15 Aug 2023
</commit_message>
<xml_diff>
--- a/Data Files/dataFile.xlsx
+++ b/Data Files/dataFile.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>User Name</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Test14082024@657</t>
+  </si>
+  <si>
+    <t>Test15082024@480.com</t>
+  </si>
+  <si>
+    <t>Test15082024@480</t>
   </si>
 </sst>
 </file>
@@ -552,10 +558,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="3"/>
     </row>

</xml_diff>